<commit_message>
test to verify if two excels are identical and removed assetId.toegekendDoor as a true fixed header
</commit_message>
<xml_diff>
--- a/UnitTests/Excel/test_file_VR_output.xlsx
+++ b/UnitTests/Excel/test_file_VR_output.xlsx
@@ -2650,7 +2650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2671,35 +2671,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>assetId.toegekendDoor</t>
+          <t>bron.typeURI</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>bron.typeURI</t>
+          <t>bronAssetId.identificator</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>bronAssetId.identificator</t>
+          <t>doel.typeURI</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>doel.typeURI</t>
+          <t>doelAssetId.identificator</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>doelAssetId.identificator</t>
+          <t>isActief</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>isActief</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>rol</t>
         </is>
@@ -2716,31 +2711,30 @@
           <t>100444c5-2a4b-4b97-8f9d-9de2969ab463-b25kZXJkZWVsI0hlZWZ0QmV0cm9ra2VuZQ</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Verkeersregelaar</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Verkeersregelaar</t>
+          <t>f184a415-10c3-465a-85d0-5e3495e7c57f-b25kZXJkZWVsI1ZlcmtlZXJzcmVnZWxhYXI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>f184a415-10c3-465a-85d0-5e3495e7c57f-b25kZXJkZWVsI1ZlcmtlZXJzcmVnZWxhYXI</t>
+          <t>http://purl.org/dc/terms/Agent</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/Agent</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>f7702193-ab88-42fb-a97d-fcb0181d9faa-cHVybDpBZ2VudA</t>
         </is>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>toezichter</t>
         </is>

</xml_diff>